<commit_message>
Add a sintonization function
</commit_message>
<xml_diff>
--- a/myPaper/motorModel/RPMdata1.xlsx
+++ b/myPaper/motorModel/RPMdata1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Satellite_Attitude_Control\myPaper\motorModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDF399E-4AAB-401D-B234-02400CCA8D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4820171-058B-4FE0-AF3C-C3E165E7F499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBD538D8-42F5-4C62-86D7-92F97027E170}"/>
   </bookViews>
@@ -16,43 +16,26 @@
     <sheet name="1second" sheetId="1" r:id="rId1"/>
     <sheet name="5samples" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'1second'!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'1second'!$A$2:$A$801</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'1second'!$F$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'1second'!$F$2:$F$801</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'1second'!$A$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'1second'!$A$2:$A$801</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'1second'!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'1second'!$B$2:$B$801</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'1second'!$C$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'1second'!$C$2:$C$801</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'1second'!$D$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'1second'!$D$2:$D$801</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'1second'!$B$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'1second'!$E$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'1second'!$E$2:$E$801</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'1second'!$F$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'1second'!$F$2:$F$801</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'1second'!$B$2:$B$801</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'1second'!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'1second'!$C$2:$C$801</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'1second'!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'1second'!$D$2:$D$801</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'1second'!$E$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'1second'!$E$2:$E$801</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Velocidad (rpm)</t>
   </si>
@@ -63,13 +46,22 @@
     <t>time(s)</t>
   </si>
   <si>
-    <t>Current (A)</t>
+    <t>Input_PWM</t>
   </si>
   <si>
-    <t>Potencia (W)</t>
+    <t>time_s</t>
   </si>
   <si>
-    <t>Current Pasos</t>
+    <t>Current_A</t>
+  </si>
+  <si>
+    <t>Potencia_W</t>
+  </si>
+  <si>
+    <t>Current_Pasos_A</t>
+  </si>
+  <si>
+    <t>Velocidad_rpm</t>
   </si>
 </sst>
 </file>
@@ -461,7 +453,7 @@
   <dimension ref="A1:F801"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,22 +466,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>